<commit_message>
Create Лист Microsoft Excel.xlsx
</commit_message>
<xml_diff>
--- a/pyrrr/Лист Microsoft Excel.xlsx
+++ b/pyrrr/Лист Microsoft Excel.xlsx
@@ -353,14 +353,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>